<commit_message>
updates with more decimal points to fix rounding error on proportions xlxs
</commit_message>
<xml_diff>
--- a/Deliverables/12S/regions/arctic/ADFG_12s_arctic_speciesxsamples.xlsx
+++ b/Deliverables/12S/regions/arctic/ADFG_12s_arctic_speciesxsamples.xlsx
@@ -1,279 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29530"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MBall\OneDrive\Documents\UW-DOCS\WADE lab\Arctic-predator-diet-microbiome\Deliverables\12S\regions\arctic\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0C30F6-0B3B-40E4-9689-84D911C83DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="absolute_abundance" sheetId="1" r:id="rId1"/>
     <sheet name="proportional_abundance" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="82">
-  <si>
-    <t>LabID</t>
-  </si>
-  <si>
-    <t>Specimen.ID</t>
-  </si>
-  <si>
-    <t>Eleginus gracilis</t>
-  </si>
-  <si>
-    <t>Clupea pallasii</t>
-  </si>
-  <si>
-    <t>Osmerus mordax</t>
-  </si>
-  <si>
-    <t>Myoxocephalus spp.</t>
-  </si>
-  <si>
-    <t>Ammodytes hexapterus</t>
-  </si>
-  <si>
-    <t>ASV16</t>
-  </si>
-  <si>
-    <t>Gymnocanthus spp.</t>
-  </si>
-  <si>
-    <t>Liparis spp.</t>
-  </si>
-  <si>
-    <t>Leptoclinus maculatus</t>
-  </si>
-  <si>
-    <t>Gymnocanthus tricuspis</t>
-  </si>
-  <si>
-    <t>Platichthys stellatus</t>
-  </si>
-  <si>
-    <t>Gadus chalcogrammus</t>
-  </si>
-  <si>
-    <t>Hemilepidotus spp.</t>
-  </si>
-  <si>
-    <t>Boreogadus saida</t>
-  </si>
-  <si>
-    <t>Lepidopsetta spp.</t>
-  </si>
-  <si>
-    <t>Liparis tunicatus</t>
-  </si>
-  <si>
-    <t>Stichaeus punctatus</t>
-  </si>
-  <si>
-    <t>Pleuronectes quadrituberculatus</t>
-  </si>
-  <si>
-    <t>ASV87</t>
-  </si>
-  <si>
-    <t>Nautichthys pribilovius</t>
-  </si>
-  <si>
-    <t>Acantholumpenus mackayi</t>
-  </si>
-  <si>
-    <t>ASV117</t>
-  </si>
-  <si>
-    <t>Gadus spp.</t>
-  </si>
-  <si>
-    <t>WADE-003-019</t>
-  </si>
-  <si>
-    <t>2021BDL-0708Sa</t>
-  </si>
-  <si>
-    <t>WADE-003-020</t>
-  </si>
-  <si>
-    <t>2021BDL-0723A</t>
-  </si>
-  <si>
-    <t>WADE-003-034</t>
-  </si>
-  <si>
-    <t>DL21OTZ007</t>
-  </si>
-  <si>
-    <t>WADE-003-040</t>
-  </si>
-  <si>
-    <t>DL22OTZ004</t>
-  </si>
-  <si>
-    <t>WADE-003-104</t>
-  </si>
-  <si>
-    <t>EB23PH005-S</t>
-  </si>
-  <si>
-    <t>WADE-003-109</t>
-  </si>
-  <si>
-    <t>EB24GAM027-S</t>
-  </si>
-  <si>
-    <t>WADE-003-110</t>
-  </si>
-  <si>
-    <t>EB24PH055-S</t>
-  </si>
-  <si>
-    <t>WADE-003-111</t>
-  </si>
-  <si>
-    <t>EB24PH075-S</t>
-  </si>
-  <si>
-    <t>WADE-003-124</t>
-  </si>
-  <si>
-    <t>WADE-003-112</t>
-  </si>
-  <si>
-    <t>PH22SH004-S</t>
-  </si>
-  <si>
-    <t>WADE-003-113</t>
-  </si>
-  <si>
-    <t>PH22SH005-S</t>
-  </si>
-  <si>
-    <t>WADE-003-114</t>
-  </si>
-  <si>
-    <t>PH22SH015-S</t>
-  </si>
-  <si>
-    <t>WADE-003-123</t>
-  </si>
-  <si>
-    <t>PH22SH036-S</t>
-  </si>
-  <si>
-    <t>WADE-003-116</t>
-  </si>
-  <si>
-    <t>PH22SH043-S</t>
-  </si>
-  <si>
-    <t>WADE-003-118</t>
-  </si>
-  <si>
-    <t>PH23SH005-S</t>
-  </si>
-  <si>
-    <t>WADE-003-120</t>
-  </si>
-  <si>
-    <t>PH23SH032-S</t>
-  </si>
-  <si>
-    <t>WADE-003-125</t>
-  </si>
-  <si>
-    <t>EB21GAM031-F</t>
-  </si>
-  <si>
-    <t>WADE-003-127</t>
-  </si>
-  <si>
-    <t>EB23PH005-F</t>
-  </si>
-  <si>
-    <t>WADE-003-129</t>
-  </si>
-  <si>
-    <t>EB23SH008-F</t>
-  </si>
-  <si>
-    <t>WADE-003-130</t>
-  </si>
-  <si>
-    <t>EB23SH009-F</t>
-  </si>
-  <si>
-    <t>WADE-003-131</t>
-  </si>
-  <si>
-    <t>EB24GAM020-F</t>
-  </si>
-  <si>
-    <t>WADE-003-134</t>
-  </si>
-  <si>
-    <t>EB24PH075-F</t>
-  </si>
-  <si>
-    <t>WADE-003-135</t>
-  </si>
-  <si>
-    <t>PH22SH004-F</t>
-  </si>
-  <si>
-    <t>WADE-003-136</t>
-  </si>
-  <si>
-    <t>PH22SH005-F</t>
-  </si>
-  <si>
-    <t>WADE-003-137</t>
-  </si>
-  <si>
-    <t>PH22SH015-F</t>
-  </si>
-  <si>
-    <t>WADE-003-139</t>
-  </si>
-  <si>
-    <t>PH22SH043-F</t>
-  </si>
-  <si>
-    <t>WADE-003-141</t>
-  </si>
-  <si>
-    <t>PH23SH005-F</t>
-  </si>
-  <si>
-    <t>WADE-003-143</t>
-  </si>
-  <si>
-    <t>PH23SH032-F</t>
-  </si>
-  <si>
-    <t>WADE-003-144</t>
-  </si>
-  <si>
-    <t>PH24GAM014-F</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,21 +64,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -373,7 +108,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -407,7 +142,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -442,10 +176,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -618,121 +351,150 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.53125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.06640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.9296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.06640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.1328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.19921875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.59765625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.9296875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.73046875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LabID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Specimen.ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Eleginus gracilis</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Clupea pallasii</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Osmerus mordax</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Myoxocephalus spp.</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Ammodytes hexapterus</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ASV16</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Gymnocanthus spp.</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Liparis spp.</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Leptoclinus maculatus</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Gymnocanthus tricuspis</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Platichthys stellatus</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Gadus chalcogrammus</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Hemilepidotus spp.</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Boreogadus saida</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Lepidopsetta spp.</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Liparis tunicatus</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Stichaeus punctatus</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Pleuronectes quadrituberculatus</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>ASV87</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Nautichthys pribilovius</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Acantholumpenus mackayi</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>ASV117</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Gadus spp.</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>WADE-003-019</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2021BDL-0708Sa</t>
+        </is>
       </c>
       <c r="C2">
         <v>16233</v>
@@ -804,12 +566,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>WADE-003-020</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2021BDL-0723A</t>
+        </is>
       </c>
       <c r="C3">
         <v>0</v>
@@ -881,12 +647,16 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>WADE-003-034</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>DL21OTZ007</t>
+        </is>
       </c>
       <c r="C4">
         <v>6397</v>
@@ -958,12 +728,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>WADE-003-040</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>DL22OTZ004</t>
+        </is>
       </c>
       <c r="C5">
         <v>270</v>
@@ -1035,12 +809,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>WADE-003-104</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>EB23PH005-S</t>
+        </is>
       </c>
       <c r="C6">
         <v>9099</v>
@@ -1112,12 +890,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>WADE-003-109</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>EB24GAM027-S</t>
+        </is>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1189,12 +971,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>WADE-003-110</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>EB24PH055-S</t>
+        </is>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1266,12 +1052,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" t="s">
-        <v>40</v>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>WADE-003-111</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>EB24PH075-S</t>
+        </is>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1292,7 +1082,7 @@
         <v>762</v>
       </c>
       <c r="I9">
-        <v>405</v>
+        <v>412</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1343,12 +1133,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" t="s">
-        <v>40</v>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>WADE-003-124</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>EB24PH075-S</t>
+        </is>
       </c>
       <c r="C10">
         <v>3</v>
@@ -1420,12 +1214,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" t="s">
-        <v>43</v>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>WADE-003-112</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>PH22SH004-S</t>
+        </is>
       </c>
       <c r="C11">
         <v>132972</v>
@@ -1497,12 +1295,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" t="s">
-        <v>45</v>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>WADE-003-113</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>PH22SH005-S</t>
+        </is>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1574,12 +1376,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" t="s">
-        <v>47</v>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>WADE-003-114</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>PH22SH015-S</t>
+        </is>
       </c>
       <c r="C13">
         <v>332771</v>
@@ -1651,12 +1457,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" t="s">
-        <v>49</v>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>WADE-003-123</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>PH22SH036-S</t>
+        </is>
       </c>
       <c r="C14">
         <v>33199</v>
@@ -1728,12 +1538,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" t="s">
-        <v>51</v>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>WADE-003-116</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>PH22SH043-S</t>
+        </is>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1805,12 +1619,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" t="s">
-        <v>53</v>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>WADE-003-118</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>PH23SH005-S</t>
+        </is>
       </c>
       <c r="C16">
         <v>0</v>
@@ -1882,12 +1700,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" t="s">
-        <v>55</v>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>WADE-003-120</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>PH23SH032-S</t>
+        </is>
       </c>
       <c r="C17">
         <v>8623</v>
@@ -1959,12 +1781,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" t="s">
-        <v>57</v>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>WADE-003-125</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>EB21GAM031-F</t>
+        </is>
       </c>
       <c r="C18">
         <v>0</v>
@@ -2036,12 +1862,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" t="s">
-        <v>59</v>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>WADE-003-127</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>EB23PH005-F</t>
+        </is>
       </c>
       <c r="C19">
         <v>1591</v>
@@ -2113,12 +1943,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" t="s">
-        <v>61</v>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>WADE-003-129</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>EB23SH008-F</t>
+        </is>
       </c>
       <c r="C20">
         <v>555</v>
@@ -2190,12 +2024,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" t="s">
-        <v>63</v>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>WADE-003-130</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>EB23SH009-F</t>
+        </is>
       </c>
       <c r="C21">
         <v>0</v>
@@ -2267,12 +2105,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" t="s">
-        <v>65</v>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>WADE-003-131</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>EB24GAM020-F</t>
+        </is>
       </c>
       <c r="C22">
         <v>0</v>
@@ -2344,12 +2186,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" t="s">
-        <v>67</v>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>WADE-003-134</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>EB24PH075-F</t>
+        </is>
       </c>
       <c r="C23">
         <v>235</v>
@@ -2421,12 +2267,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" t="s">
-        <v>69</v>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>WADE-003-135</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>PH22SH004-F</t>
+        </is>
       </c>
       <c r="C24">
         <v>4082</v>
@@ -2498,12 +2348,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" t="s">
-        <v>71</v>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>WADE-003-136</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>PH22SH005-F</t>
+        </is>
       </c>
       <c r="C25">
         <v>116</v>
@@ -2575,12 +2429,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" t="s">
-        <v>73</v>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>WADE-003-137</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>PH22SH015-F</t>
+        </is>
       </c>
       <c r="C26">
         <v>7877</v>
@@ -2652,12 +2510,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" t="s">
-        <v>75</v>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>WADE-003-139</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>PH22SH043-F</t>
+        </is>
       </c>
       <c r="C27">
         <v>137</v>
@@ -2729,12 +2591,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>76</v>
-      </c>
-      <c r="B28" t="s">
-        <v>77</v>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>WADE-003-141</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>PH23SH005-F</t>
+        </is>
       </c>
       <c r="C28">
         <v>8099</v>
@@ -2806,12 +2672,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29" t="s">
-        <v>79</v>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>WADE-003-143</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>PH23SH032-F</t>
+        </is>
       </c>
       <c r="C29">
         <v>124</v>
@@ -2883,12 +2753,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30" t="s">
-        <v>81</v>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>WADE-003-144</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>PH24GAM014-F</t>
+        </is>
       </c>
       <c r="C30">
         <v>0</v>
@@ -2966,132 +2840,162 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.53125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.06640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.9296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.06640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.1328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.19921875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.59765625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.9296875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.73046875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>LabID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Specimen.ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Eleginus gracilis</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Clupea pallasii</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Osmerus mordax</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Myoxocephalus spp.</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Ammodytes hexapterus</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ASV16</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Gymnocanthus spp.</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Liparis spp.</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Leptoclinus maculatus</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Gymnocanthus tricuspis</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Platichthys stellatus</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Gadus chalcogrammus</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Hemilepidotus spp.</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Boreogadus saida</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Lepidopsetta spp.</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Liparis tunicatus</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Stichaeus punctatus</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Pleuronectes quadrituberculatus</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>ASV87</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Nautichthys pribilovius</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Acantholumpenus mackayi</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>ASV117</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Gadus spp.</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>WADE-003-019</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2021BDL-0708Sa</t>
+        </is>
       </c>
       <c r="C2">
-        <v>0.85399999999999998</v>
+        <v>0.85356</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.00026</v>
       </c>
       <c r="F2">
-        <v>0.14499999999999999</v>
+        <v>0.1446</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -3121,7 +3025,7 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>2E-3</v>
+        <v>0.00158</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -3151,12 +3055,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>WADE-003-020</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2021BDL-0723A</t>
+        </is>
       </c>
       <c r="C3">
         <v>0</v>
@@ -3171,10 +3079,10 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>1.9E-2</v>
+        <v>0.01853</v>
       </c>
       <c r="H3">
-        <v>2E-3</v>
+        <v>0.00214</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -3198,7 +3106,7 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0.95799999999999996</v>
+        <v>0.95795</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -3225,18 +3133,22 @@
         <v>0</v>
       </c>
       <c r="Y3">
-        <v>2.1000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
+        <v>0.02138</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>WADE-003-034</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>DL21OTZ007</t>
+        </is>
       </c>
       <c r="C4">
-        <v>0.99399999999999999</v>
+        <v>0.9944</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -3248,7 +3160,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>6.0000000000000001E-3</v>
+        <v>0.0056</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -3305,18 +3217,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>WADE-003-040</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>DL22OTZ004</t>
+        </is>
       </c>
       <c r="C5">
-        <v>0.96099999999999997</v>
+        <v>0.96085</v>
       </c>
       <c r="D5">
-        <v>3.9E-2</v>
+        <v>0.03915</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -3382,24 +3298,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>WADE-003-104</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>EB23PH005-S</t>
+        </is>
       </c>
       <c r="C6">
-        <v>0.52500000000000002</v>
+        <v>0.52523</v>
       </c>
       <c r="D6">
-        <v>1E-3</v>
+        <v>0.00144</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0.255</v>
+        <v>0.25508</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -3417,7 +3337,7 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0.218</v>
+        <v>0.21825</v>
       </c>
       <c r="M6">
         <v>0</v>
@@ -3459,12 +3379,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>WADE-003-109</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>EB24GAM027-S</t>
+        </is>
       </c>
       <c r="C7">
         <v>0</v>
@@ -3476,7 +3400,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0.876</v>
+        <v>0.87575</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -3488,7 +3412,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>8.0000000000000002E-3</v>
+        <v>0.00844</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -3497,7 +3421,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>3.1E-2</v>
+        <v>0.03136</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -3506,10 +3430,10 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <v>5.1999999999999998E-2</v>
+        <v>0.05187</v>
       </c>
       <c r="Q7">
-        <v>3.3000000000000002E-2</v>
+        <v>0.03257</v>
       </c>
       <c r="R7">
         <v>0</v>
@@ -3536,12 +3460,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>38</v>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>WADE-003-110</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>EB24PH055-S</t>
+        </is>
       </c>
       <c r="C8">
         <v>0</v>
@@ -3556,25 +3484,25 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>2.8000000000000001E-2</v>
+        <v>0.02841</v>
       </c>
       <c r="H8">
-        <v>0.83699999999999997</v>
+        <v>0.83652</v>
       </c>
       <c r="I8">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008399999999999999</v>
       </c>
       <c r="J8">
         <v>0</v>
       </c>
       <c r="K8">
-        <v>5.6000000000000001E-2</v>
+        <v>0.05565</v>
       </c>
       <c r="L8">
-        <v>0.01</v>
+        <v>0.01036</v>
       </c>
       <c r="M8">
-        <v>0.03</v>
+        <v>0.02957</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -3595,7 +3523,7 @@
         <v>0</v>
       </c>
       <c r="T8">
-        <v>0.02</v>
+        <v>0.02019</v>
       </c>
       <c r="U8">
         <v>0</v>
@@ -3604,7 +3532,7 @@
         <v>0</v>
       </c>
       <c r="W8">
-        <v>1.0999999999999999E-2</v>
+        <v>0.0109</v>
       </c>
       <c r="X8">
         <v>0</v>
@@ -3613,12 +3541,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" t="s">
-        <v>40</v>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>WADE-003-111</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>EB24PH075-S</t>
+        </is>
       </c>
       <c r="C9">
         <v>0</v>
@@ -3630,25 +3562,25 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.57799999999999996</v>
+        <v>0.57787</v>
       </c>
       <c r="G9">
-        <v>0.27100000000000002</v>
+        <v>0.27066</v>
       </c>
       <c r="H9">
-        <v>3.5999999999999997E-2</v>
+        <v>0.03617</v>
       </c>
       <c r="I9">
-        <v>1.9E-2</v>
+        <v>0.01956</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>6.4000000000000001E-2</v>
+        <v>0.06403</v>
       </c>
       <c r="L9">
-        <v>1.6E-2</v>
+        <v>0.01647</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -3669,7 +3601,7 @@
         <v>0</v>
       </c>
       <c r="S9">
-        <v>1.4999999999999999E-2</v>
+        <v>0.01524</v>
       </c>
       <c r="T9">
         <v>0</v>
@@ -3690,42 +3622,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" t="s">
-        <v>40</v>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>WADE-003-124</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>EB24PH075-S</t>
+        </is>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.00017</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>0.00028</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0.872</v>
+        <v>0.87153</v>
       </c>
       <c r="G10">
-        <v>0.06</v>
+        <v>0.05972</v>
       </c>
       <c r="H10">
-        <v>5.0000000000000001E-3</v>
+        <v>0.00459</v>
       </c>
       <c r="I10">
-        <v>4.4999999999999998E-2</v>
+        <v>0.04517</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>1.0999999999999999E-2</v>
+        <v>0.01057</v>
       </c>
       <c r="L10">
-        <v>3.0000000000000001E-3</v>
+        <v>0.00332</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -3746,7 +3682,7 @@
         <v>0</v>
       </c>
       <c r="S10">
-        <v>5.0000000000000001E-3</v>
+        <v>0.00465</v>
       </c>
       <c r="T10">
         <v>0</v>
@@ -3767,21 +3703,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" t="s">
-        <v>43</v>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>WADE-003-112</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>PH22SH004-S</t>
+        </is>
       </c>
       <c r="C11">
-        <v>0.13</v>
+        <v>0.13045</v>
       </c>
       <c r="D11">
-        <v>0.86899999999999999</v>
+        <v>0.86944</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>5E-05</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -3790,7 +3730,7 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>6E-05</v>
       </c>
       <c r="I11">
         <v>0</v>
@@ -3844,18 +3784,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" t="s">
-        <v>45</v>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>WADE-003-113</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>PH22SH005-S</t>
+        </is>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0.61399999999999999</v>
+        <v>0.61386</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -3867,7 +3811,7 @@
         <v>0</v>
       </c>
       <c r="H12">
-        <v>0.38600000000000001</v>
+        <v>0.38614</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -3921,21 +3865,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" t="s">
-        <v>47</v>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>WADE-003-114</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>PH22SH015-S</t>
+        </is>
       </c>
       <c r="C13">
-        <v>0.40799999999999997</v>
+        <v>0.40783</v>
       </c>
       <c r="D13">
-        <v>0.42</v>
+        <v>0.4202</v>
       </c>
       <c r="E13">
-        <v>0.17199999999999999</v>
+        <v>0.17197</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -3998,21 +3946,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" t="s">
-        <v>49</v>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>WADE-003-123</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>PH22SH036-S</t>
+        </is>
       </c>
       <c r="C14">
-        <v>0.66800000000000004</v>
+        <v>0.66812</v>
       </c>
       <c r="D14">
-        <v>0.25900000000000001</v>
+        <v>0.25862</v>
       </c>
       <c r="E14">
-        <v>7.2999999999999995E-2</v>
+        <v>0.07325</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -4075,18 +4027,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" t="s">
-        <v>51</v>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>WADE-003-116</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>PH22SH043-S</t>
+        </is>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>0.996</v>
+        <v>0.9962800000000001</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -4122,7 +4078,7 @@
         <v>0</v>
       </c>
       <c r="P15">
-        <v>4.0000000000000001E-3</v>
+        <v>0.00372</v>
       </c>
       <c r="Q15">
         <v>0</v>
@@ -4152,12 +4108,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" t="s">
-        <v>53</v>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>WADE-003-118</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>PH23SH005-S</t>
+        </is>
       </c>
       <c r="C16">
         <v>0</v>
@@ -4229,21 +4189,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" t="s">
-        <v>55</v>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>WADE-003-120</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>PH23SH032-S</t>
+        </is>
       </c>
       <c r="C17">
-        <v>0.28199999999999997</v>
+        <v>0.28167</v>
       </c>
       <c r="D17">
-        <v>0.191</v>
+        <v>0.19083</v>
       </c>
       <c r="E17">
-        <v>0.52800000000000002</v>
+        <v>0.5275</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -4306,12 +4270,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" t="s">
-        <v>57</v>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>WADE-003-125</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>EB21GAM031-F</t>
+        </is>
       </c>
       <c r="C18">
         <v>0</v>
@@ -4335,7 +4303,7 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <v>0.40400000000000003</v>
+        <v>0.40441</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -4350,7 +4318,7 @@
         <v>0</v>
       </c>
       <c r="O18">
-        <v>0.59599999999999997</v>
+        <v>0.59559</v>
       </c>
       <c r="P18">
         <v>0</v>
@@ -4383,15 +4351,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" t="s">
-        <v>59</v>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>WADE-003-127</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>EB23PH005-F</t>
+        </is>
       </c>
       <c r="C19">
-        <v>0.17899999999999999</v>
+        <v>0.17945</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -4400,22 +4372,22 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>4.1000000000000002E-2</v>
+        <v>0.04072</v>
       </c>
       <c r="G19">
         <v>0</v>
       </c>
       <c r="H19">
-        <v>6.2E-2</v>
+        <v>0.06215</v>
       </c>
       <c r="I19">
-        <v>0.47699999999999998</v>
+        <v>0.4771</v>
       </c>
       <c r="J19">
-        <v>1E-3</v>
+        <v>0.00079</v>
       </c>
       <c r="K19">
-        <v>0.23</v>
+        <v>0.23032</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -4427,7 +4399,7 @@
         <v>0</v>
       </c>
       <c r="O19">
-        <v>0</v>
+        <v>0.00045</v>
       </c>
       <c r="P19">
         <v>0</v>
@@ -4454,36 +4426,40 @@
         <v>0</v>
       </c>
       <c r="X19">
-        <v>8.9999999999999993E-3</v>
+        <v>0.00902</v>
       </c>
       <c r="Y19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" t="s">
-        <v>61</v>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>WADE-003-129</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>EB23SH008-F</t>
+        </is>
       </c>
       <c r="C20">
-        <v>5.5E-2</v>
+        <v>0.05526</v>
       </c>
       <c r="D20">
-        <v>1.7000000000000001E-2</v>
+        <v>0.01693</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
       <c r="F20">
-        <v>0.504</v>
+        <v>0.50408</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
       <c r="H20">
-        <v>3.0000000000000001E-3</v>
+        <v>0.00269</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -4498,7 +4474,7 @@
         <v>0</v>
       </c>
       <c r="M20">
-        <v>0.42</v>
+        <v>0.41995</v>
       </c>
       <c r="N20">
         <v>0</v>
@@ -4528,7 +4504,7 @@
         <v>0</v>
       </c>
       <c r="W20">
-        <v>1E-3</v>
+        <v>0.0011</v>
       </c>
       <c r="X20">
         <v>0</v>
@@ -4537,12 +4513,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" t="s">
-        <v>63</v>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>WADE-003-130</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>EB23SH009-F</t>
+        </is>
       </c>
       <c r="C21">
         <v>0</v>
@@ -4557,10 +4537,10 @@
         <v>0</v>
       </c>
       <c r="G21">
-        <v>6.0000000000000001E-3</v>
+        <v>0.00576</v>
       </c>
       <c r="H21">
-        <v>0.96399999999999997</v>
+        <v>0.96373</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -4569,7 +4549,7 @@
         <v>0</v>
       </c>
       <c r="K21">
-        <v>3.1E-2</v>
+        <v>0.03051</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -4614,12 +4594,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" t="s">
-        <v>65</v>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>WADE-003-131</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>EB24GAM020-F</t>
+        </is>
       </c>
       <c r="C22">
         <v>0</v>
@@ -4631,7 +4615,7 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>0.48199999999999998</v>
+        <v>0.48172</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -4643,7 +4627,7 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>0.34499999999999997</v>
+        <v>0.34474</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -4655,7 +4639,7 @@
         <v>0</v>
       </c>
       <c r="N22">
-        <v>1.7999999999999999E-2</v>
+        <v>0.01834</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -4664,10 +4648,10 @@
         <v>0</v>
       </c>
       <c r="Q22">
-        <v>0.10100000000000001</v>
+        <v>0.10125</v>
       </c>
       <c r="R22">
-        <v>3.5000000000000003E-2</v>
+        <v>0.035</v>
       </c>
       <c r="S22">
         <v>0</v>
@@ -4679,7 +4663,7 @@
         <v>0</v>
       </c>
       <c r="V22">
-        <v>1.9E-2</v>
+        <v>0.01895</v>
       </c>
       <c r="W22">
         <v>0</v>
@@ -4691,15 +4675,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" t="s">
-        <v>67</v>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>WADE-003-134</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>EB24PH075-F</t>
+        </is>
       </c>
       <c r="C23">
-        <v>0.03</v>
+        <v>0.03035</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -4708,13 +4696,13 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>0.40799999999999997</v>
+        <v>0.40798</v>
       </c>
       <c r="G23">
-        <v>8.7999999999999995E-2</v>
+        <v>0.08756</v>
       </c>
       <c r="H23">
-        <v>8.5999999999999993E-2</v>
+        <v>0.08575000000000001</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -4723,10 +4711,10 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <v>0.17599999999999999</v>
+        <v>0.17629</v>
       </c>
       <c r="L23">
-        <v>0.14899999999999999</v>
+        <v>0.14917</v>
       </c>
       <c r="M23">
         <v>0</v>
@@ -4753,7 +4741,7 @@
         <v>0</v>
       </c>
       <c r="U23">
-        <v>4.7E-2</v>
+        <v>0.04727</v>
       </c>
       <c r="V23">
         <v>0</v>
@@ -4762,24 +4750,28 @@
         <v>0</v>
       </c>
       <c r="X23">
-        <v>1.6E-2</v>
+        <v>0.01563</v>
       </c>
       <c r="Y23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" t="s">
-        <v>69</v>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>WADE-003-135</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>PH22SH004-F</t>
+        </is>
       </c>
       <c r="C24">
-        <v>0.23599999999999999</v>
+        <v>0.23576</v>
       </c>
       <c r="D24">
-        <v>0.76400000000000001</v>
+        <v>0.76424</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -4845,15 +4837,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" t="s">
-        <v>71</v>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>WADE-003-136</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>PH22SH005-F</t>
+        </is>
       </c>
       <c r="C25">
-        <v>1.2999999999999999E-2</v>
+        <v>0.01296</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -4865,7 +4861,7 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <v>0.874</v>
+        <v>0.87374</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -4877,7 +4873,7 @@
         <v>0</v>
       </c>
       <c r="K25">
-        <v>1E-3</v>
+        <v>0.00078</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -4886,7 +4882,7 @@
         <v>0</v>
       </c>
       <c r="N25">
-        <v>0.113</v>
+        <v>0.11251</v>
       </c>
       <c r="O25">
         <v>0</v>
@@ -4922,33 +4918,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" t="s">
-        <v>73</v>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>WADE-003-137</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>PH22SH015-F</t>
+        </is>
       </c>
       <c r="C26">
-        <v>0.66300000000000003</v>
+        <v>0.66316</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>0.14499999999999999</v>
+        <v>0.14523</v>
       </c>
       <c r="F26">
-        <v>1E-3</v>
+        <v>0.0009300000000000001</v>
       </c>
       <c r="G26">
-        <v>3.0000000000000001E-3</v>
+        <v>0.00278</v>
       </c>
       <c r="H26">
-        <v>4.2999999999999997E-2</v>
+        <v>0.04302</v>
       </c>
       <c r="I26">
-        <v>6.5000000000000002E-2</v>
+        <v>0.06499000000000001</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -4960,7 +4960,7 @@
         <v>0</v>
       </c>
       <c r="M26">
-        <v>3.0000000000000001E-3</v>
+        <v>0.00295</v>
       </c>
       <c r="N26">
         <v>0</v>
@@ -4969,7 +4969,7 @@
         <v>0</v>
       </c>
       <c r="P26">
-        <v>3.3000000000000002E-2</v>
+        <v>0.03334</v>
       </c>
       <c r="Q26">
         <v>0</v>
@@ -4978,10 +4978,10 @@
         <v>0</v>
       </c>
       <c r="S26">
-        <v>1.0999999999999999E-2</v>
+        <v>0.01069</v>
       </c>
       <c r="T26">
-        <v>2.7E-2</v>
+        <v>0.02702</v>
       </c>
       <c r="U26">
         <v>0</v>
@@ -4993,30 +4993,34 @@
         <v>0</v>
       </c>
       <c r="X26">
-        <v>6.0000000000000001E-3</v>
+        <v>0.00589</v>
       </c>
       <c r="Y26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" t="s">
-        <v>75</v>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>WADE-003-139</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>PH22SH043-F</t>
+        </is>
       </c>
       <c r="C27">
-        <v>1.2999999999999999E-2</v>
+        <v>0.01339</v>
       </c>
       <c r="D27">
-        <v>0.9</v>
+        <v>0.90024</v>
       </c>
       <c r="E27">
-        <v>0.06</v>
+        <v>0.06028</v>
       </c>
       <c r="F27">
-        <v>2.5999999999999999E-2</v>
+        <v>0.02609</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -5076,30 +5080,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>76</v>
-      </c>
-      <c r="B28" t="s">
-        <v>77</v>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>WADE-003-141</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>PH23SH005-F</t>
+        </is>
       </c>
       <c r="C28">
-        <v>0.375</v>
+        <v>0.37518</v>
       </c>
       <c r="D28">
-        <v>0.59399999999999997</v>
+        <v>0.59406</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>2.5000000000000001E-2</v>
+        <v>0.02548</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28">
-        <v>5.0000000000000001E-3</v>
+        <v>0.00528</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -5153,21 +5161,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29" t="s">
-        <v>79</v>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>WADE-003-143</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>PH23SH032-F</t>
+        </is>
       </c>
       <c r="C29">
-        <v>0.39100000000000001</v>
+        <v>0.39117</v>
       </c>
       <c r="D29">
-        <v>0.45100000000000001</v>
+        <v>0.4511</v>
       </c>
       <c r="E29">
-        <v>0.158</v>
+        <v>0.15773</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -5230,12 +5242,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30" t="s">
-        <v>81</v>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>WADE-003-144</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>PH24GAM014-F</t>
+        </is>
       </c>
       <c r="C30">
         <v>0</v>

</xml_diff>